<commit_message>
REPORTGEN-1154: fix templates for PCI DSS V3.1 and V3.2.1 + add new templates for PCI DSS V4
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Compliance reports/PCI-DSS-V3.1 Full Detailed Report.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Compliance reports/PCI-DSS-V3.1 Full Detailed Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8176375-DC3D-421B-8E11-2DEB2F8EBE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76B0524-7C86-4840-AFF0-29EADA6F4AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -270,7 +270,7 @@
     <t>RepGen:TEXT;OMG_TECHNICAL_DEBT</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=PCI-DSS-V3.1,MORE=true,HEADER=NO,EVOLUTION=true</t>
+    <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=PCI-DSS-V3.1,HEADER=NO,EVOLUTION=true</t>
   </si>
 </sst>
 </file>
@@ -501,16 +501,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -520,10 +520,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -931,26 +931,26 @@
   <dimension ref="B1:O14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" customWidth="1"/>
-    <col min="2" max="2" width="75.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="75.28515625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="36.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="36.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
@@ -960,7 +960,7 @@
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
     </row>
-    <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
@@ -970,7 +970,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
         <v>0</v>
       </c>
@@ -986,7 +986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="22" t="s">
         <v>1</v>
       </c>
@@ -1002,10 +1002,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>8</v>
       </c>
@@ -1016,13 +1016,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>31</v>
       </c>
       <c r="D7" s="23"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" s="18" t="s">
         <v>32</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>34</v>
       </c>
@@ -1038,12 +1038,12 @@
       <c r="N9" s="17"/>
       <c r="O9" s="16"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B13" s="19" t="s">
         <v>35</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>71</v>
       </c>
@@ -1083,21 +1083,21 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="59.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="59.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>39</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>59</v>
       </c>
@@ -1145,24 +1145,24 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="99.44140625" customWidth="1"/>
-    <col min="2" max="2" width="59.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="99.42578125" customWidth="1"/>
+    <col min="2" max="2" width="59.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1207,21 +1207,21 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="44.44140625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>39</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>61</v>
       </c>
@@ -1269,24 +1269,24 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="106.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="106.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1331,21 +1331,21 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="44.44140625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>39</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>63</v>
       </c>
@@ -1393,24 +1393,24 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="98.44140625" customWidth="1"/>
+    <col min="1" max="1" width="98.42578125" customWidth="1"/>
     <col min="2" max="2" width="70" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -1455,21 +1455,21 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="85.88671875" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="85.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="46.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>39</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>65</v>
       </c>
@@ -1517,24 +1517,24 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="108.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="108.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1579,21 +1579,21 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="44.44140625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>39</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>67</v>
       </c>
@@ -1641,24 +1641,24 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="100.33203125" customWidth="1"/>
-    <col min="2" max="2" width="77.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="100.28515625" customWidth="1"/>
+    <col min="2" max="2" width="77.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -1703,21 +1703,21 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="44.44140625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>39</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>43</v>
       </c>
@@ -1765,24 +1765,24 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="99" customWidth="1"/>
-    <col min="2" max="2" width="60.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1827,21 +1827,21 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>39</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>53</v>
       </c>
@@ -1889,24 +1889,24 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="98.88671875" customWidth="1"/>
-    <col min="2" max="2" width="47.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.109375" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="98.85546875" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1951,21 +1951,21 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="85.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="85.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>39</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>55</v>
       </c>
@@ -2013,24 +2013,24 @@
       <selection activeCell="A11" sqref="A10:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="99.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="99.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -2075,21 +2075,21 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>39</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>57</v>
       </c>
@@ -2137,24 +2137,24 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="99.33203125" customWidth="1"/>
-    <col min="2" max="2" width="87.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="99.28515625" customWidth="1"/>
+    <col min="2" max="2" width="87.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>

</xml_diff>